<commit_message>
first version of the report
</commit_message>
<xml_diff>
--- a/Dataset/Dataset.xlsx
+++ b/Dataset/Dataset.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aesops\DTE-Datathon\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA42E9D-ED8E-4BCB-A88A-B550BED0281A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C137E53-668C-4B2D-830E-50CAD30C8909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
-    <sheet name="data" sheetId="1" r:id="rId2"/>
-    <sheet name="population distribution" sheetId="2" r:id="rId3"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="population distribution" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'population distribution'!$A$1:$E$236</definedName>
-    <definedName name="Z_94835D04_D966_4448_B29D_63E064533BCB_.wvu.FilterData" localSheetId="1" hidden="1">data!$A$1:$AC$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'population distribution'!$A$1:$E$236</definedName>
+    <definedName name="Z_94835D04_D966_4448_B29D_63E064533BCB_.wvu.FilterData" localSheetId="0" hidden="1">data!$A$1:$AC$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{94835D04-D966-4448-B29D-63E064533BCB}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="91">
   <si>
     <t>Country</t>
   </si>
@@ -316,6 +316,9 @@
   <si>
     <t>Count of County</t>
   </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
 </sst>
 </file>
 
@@ -493,7 +496,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kamau Kamau" refreshedDate="45195.486972222221" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="47" xr:uid="{80809D39-294C-4827-97BC-A11BB511581E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kamau Kamau" refreshedDate="45195.77226539352" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="47" xr:uid="{9AA87779-8E24-455E-8E77-87137FC0CBA5}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:AC48" sheet="data"/>
   </cacheSource>
@@ -502,7 +505,55 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="County" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="47">
+        <s v="Baringo"/>
+        <s v="Bomet"/>
+        <s v="Bungoma"/>
+        <s v="Busia"/>
+        <s v="Elgeiyo-Marakwet"/>
+        <s v="Embu"/>
+        <s v="Garissa"/>
+        <s v="Homa Bay"/>
+        <s v="Isiolo"/>
+        <s v="Kajiado"/>
+        <s v="Kakamega"/>
+        <s v="Kericho"/>
+        <s v="Kiambu"/>
+        <s v="Kilifi"/>
+        <s v="Kirinyaga"/>
+        <s v="Kisii"/>
+        <s v="Kisumu"/>
+        <s v="Kitui"/>
+        <s v="Kwale"/>
+        <s v="Laikipia"/>
+        <s v="Lamu"/>
+        <s v="Machakos"/>
+        <s v="Makueni"/>
+        <s v="Mandera"/>
+        <s v="Marsabit"/>
+        <s v="Meru"/>
+        <s v="Migori"/>
+        <s v="Mombasa"/>
+        <s v="Murang'a"/>
+        <s v="Nairobi"/>
+        <s v="Nakuru"/>
+        <s v="Nandi"/>
+        <s v="Narok"/>
+        <s v="Nyamira"/>
+        <s v="Nyandarua"/>
+        <s v="Nyeri"/>
+        <s v="Samburu"/>
+        <s v="Siaya"/>
+        <s v="Taita Taveta"/>
+        <s v="Tana River"/>
+        <s v="Tharaka - Nithi"/>
+        <s v="Trans Nzoia"/>
+        <s v="Turkana"/>
+        <s v="Uasin Gishu"/>
+        <s v="Vihiga"/>
+        <s v="Wajir"/>
+        <s v="West Pokot"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Rural_ppn" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1682239"/>
@@ -601,7 +652,7 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="47">
   <r>
     <s v="Kenya"/>
-    <s v="Baringo"/>
+    <x v="0"/>
     <n v="591474"/>
     <n v="75289"/>
     <n v="666763"/>
@@ -632,7 +683,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Bomet"/>
+    <x v="1"/>
     <n v="847718"/>
     <n v="27971"/>
     <n v="875689"/>
@@ -663,7 +714,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Bungoma"/>
+    <x v="2"/>
     <n v="1480458"/>
     <n v="190112"/>
     <n v="1670570"/>
@@ -694,7 +745,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Busia"/>
+    <x v="3"/>
     <n v="779928"/>
     <n v="113753"/>
     <n v="893681"/>
@@ -725,7 +776,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Elgeiyo-Marakwet"/>
+    <x v="4"/>
     <n v="433901"/>
     <n v="20579"/>
     <n v="454480"/>
@@ -756,7 +807,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Embu"/>
+    <x v="5"/>
     <n v="532675"/>
     <n v="75924"/>
     <n v="608599"/>
@@ -787,7 +838,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Garissa"/>
+    <x v="6"/>
     <n v="630463"/>
     <n v="210890"/>
     <n v="841353"/>
@@ -818,7 +869,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Homa Bay"/>
+    <x v="7"/>
     <n v="1018871"/>
     <n v="113079"/>
     <n v="1131950"/>
@@ -849,7 +900,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Isiolo"/>
+    <x v="8"/>
     <n v="142333"/>
     <n v="125669"/>
     <n v="268002"/>
@@ -880,7 +931,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kajiado"/>
+    <x v="9"/>
     <n v="495218"/>
     <n v="622622"/>
     <n v="1117840"/>
@@ -911,7 +962,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kakamega"/>
+    <x v="10"/>
     <n v="1682239"/>
     <n v="185340"/>
     <n v="1867579"/>
@@ -942,7 +993,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kericho"/>
+    <x v="11"/>
     <n v="808239"/>
     <n v="93538"/>
     <n v="901777"/>
@@ -973,7 +1024,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kiambu"/>
+    <x v="12"/>
     <n v="711450"/>
     <n v="1706285"/>
     <n v="2417735"/>
@@ -1004,7 +1055,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kilifi"/>
+    <x v="13"/>
     <n v="1059899"/>
     <n v="393888"/>
     <n v="1453787"/>
@@ -1035,7 +1086,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kirinyaga"/>
+    <x v="14"/>
     <n v="474187"/>
     <n v="136224"/>
     <n v="610411"/>
@@ -1066,7 +1117,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kisii"/>
+    <x v="15"/>
     <n v="1115450"/>
     <n v="151410"/>
     <n v="1266860"/>
@@ -1097,12 +1148,12 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kisumu"/>
+    <x v="16"/>
     <n v="714668"/>
     <n v="440906"/>
     <n v="1155574"/>
     <n v="0.38154717915079434"/>
-    <x v="1"/>
+    <x v="0"/>
     <n v="2086"/>
     <n v="554"/>
     <n v="7"/>
@@ -1128,7 +1179,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kitui"/>
+    <x v="17"/>
     <n v="1082168"/>
     <n v="54019"/>
     <n v="1136187"/>
@@ -1159,7 +1210,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Kwale"/>
+    <x v="18"/>
     <n v="740389"/>
     <n v="126431"/>
     <n v="866820"/>
@@ -1190,7 +1241,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Laikipia"/>
+    <x v="19"/>
     <n v="391200"/>
     <n v="127360"/>
     <n v="518560"/>
@@ -1221,7 +1272,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Lamu"/>
+    <x v="20"/>
     <n v="105474"/>
     <n v="38446"/>
     <n v="143920"/>
@@ -1252,7 +1303,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Machakos"/>
+    <x v="21"/>
     <n v="1007854"/>
     <n v="414078"/>
     <n v="1421932"/>
@@ -1283,7 +1334,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Makueni"/>
+    <x v="22"/>
     <n v="910577"/>
     <n v="77076"/>
     <n v="987653"/>
@@ -1314,12 +1365,12 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Mandera"/>
+    <x v="23"/>
     <n v="596990"/>
     <n v="270467"/>
     <n v="867457"/>
     <n v="0.31179297648183135"/>
-    <x v="1"/>
+    <x v="0"/>
     <n v="25991"/>
     <n v="33"/>
     <n v="7"/>
@@ -1345,7 +1396,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Marsabit"/>
+    <x v="24"/>
     <n v="352546"/>
     <n v="107239"/>
     <n v="459785"/>
@@ -1376,7 +1427,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Meru"/>
+    <x v="25"/>
     <n v="1406796"/>
     <n v="138918"/>
     <n v="1545714"/>
@@ -1407,7 +1458,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Migori"/>
+    <x v="26"/>
     <n v="949236"/>
     <n v="167200"/>
     <n v="1116436"/>
@@ -1438,7 +1489,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Mombasa"/>
+    <x v="27"/>
     <n v="0"/>
     <n v="1208333"/>
     <n v="1208333"/>
@@ -1469,7 +1520,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Murang'a"/>
+    <x v="28"/>
     <n v="938213"/>
     <n v="118427"/>
     <n v="1056640"/>
@@ -1500,7 +1551,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Nairobi"/>
+    <x v="29"/>
     <n v="0"/>
     <n v="4397073"/>
     <n v="4397073"/>
@@ -1531,7 +1582,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Nakuru"/>
+    <x v="30"/>
     <n v="1115122"/>
     <n v="1047080"/>
     <n v="2162202"/>
@@ -1562,7 +1613,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Nandi"/>
+    <x v="31"/>
     <n v="826232"/>
     <n v="59479"/>
     <n v="885711"/>
@@ -1593,7 +1644,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Narok"/>
+    <x v="32"/>
     <n v="1057521"/>
     <n v="100352"/>
     <n v="1157873"/>
@@ -1624,7 +1675,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Nyamira"/>
+    <x v="33"/>
     <n v="558540"/>
     <n v="47036"/>
     <n v="605576"/>
@@ -1655,7 +1706,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Nyandarua"/>
+    <x v="34"/>
     <n v="571754"/>
     <n v="66535"/>
     <n v="638289"/>
@@ -1686,7 +1737,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Nyeri"/>
+    <x v="35"/>
     <n v="608409"/>
     <n v="150755"/>
     <n v="759164"/>
@@ -1717,7 +1768,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Samburu"/>
+    <x v="36"/>
     <n v="263195"/>
     <n v="47132"/>
     <n v="310327"/>
@@ -1748,7 +1799,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Siaya"/>
+    <x v="37"/>
     <n v="907766"/>
     <n v="85417"/>
     <n v="993183"/>
@@ -1779,12 +1830,12 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Taita Taveta"/>
+    <x v="38"/>
     <n v="246897"/>
     <n v="93774"/>
     <n v="340671"/>
     <n v="0.27526264343017165"/>
-    <x v="1"/>
+    <x v="0"/>
     <n v="17084"/>
     <n v="20"/>
     <n v="4"/>
@@ -1810,7 +1861,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Tana River"/>
+    <x v="39"/>
     <n v="240221"/>
     <n v="75722"/>
     <n v="315943"/>
@@ -1841,7 +1892,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Tharaka - Nithi"/>
+    <x v="40"/>
     <n v="360434"/>
     <n v="32743"/>
     <n v="393177"/>
@@ -1872,7 +1923,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Trans Nzoia"/>
+    <x v="41"/>
     <n v="811607"/>
     <n v="178734"/>
     <n v="990341"/>
@@ -1903,7 +1954,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Turkana"/>
+    <x v="42"/>
     <n v="786185"/>
     <n v="140791"/>
     <n v="926976"/>
@@ -1934,7 +1985,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Uasin Gishu"/>
+    <x v="43"/>
     <n v="652981"/>
     <n v="510205"/>
     <n v="1163186"/>
@@ -1965,7 +2016,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Vihiga"/>
+    <x v="44"/>
     <n v="531629"/>
     <n v="58384"/>
     <n v="590013"/>
@@ -1996,7 +2047,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="Wajir"/>
+    <x v="45"/>
     <n v="604089"/>
     <n v="177174"/>
     <n v="781263"/>
@@ -2027,7 +2078,7 @@
   </r>
   <r>
     <s v="Kenya"/>
-    <s v="West Pokot"/>
+    <x v="46"/>
     <n v="107572"/>
     <n v="8610"/>
     <n v="116182"/>
@@ -2060,16 +2111,67 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AF3B326-10E9-420C-A900-75063FCFA7AE}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A46ADEC-2704-42EB-813A-FE6DD83CC3BC}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="29">
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="48">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField numFmtId="3" showAll="0"/>
     <pivotField numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -2100,9 +2202,158 @@
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="48">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
     <field x="6"/>
-  </rowFields>
-  <rowItems count="3">
+  </colFields>
+  <colItems count="3">
     <i>
       <x/>
     </i>
@@ -2112,9 +2363,6 @@
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Count of County" fld="1" subtotal="count" baseField="0" baseItem="0"/>
@@ -2328,57 +2576,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89C319D-8A7D-4689-870C-FF2B0750341B}">
-  <dimension ref="A3:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2">
-      <c r="A3" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="34">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="34">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2386,10 +2583,10 @@
   <dimension ref="A1:AE1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2519,7 +2716,7 @@
         <v>0.11291718346698902</v>
       </c>
       <c r="G2" s="30" t="str">
-        <f>IF(F2&gt;0.3,"Urban","Rural")</f>
+        <f>IF(F2&gt;0.4,"Urban","Rural")</f>
         <v>Rural</v>
       </c>
       <c r="H2" s="4">
@@ -2612,7 +2809,7 @@
         <v>3.1941705331459E-2</v>
       </c>
       <c r="G3" s="30" t="str">
-        <f t="shared" ref="G3:G48" si="2">IF(F3&gt;0.3,"Urban","Rural")</f>
+        <f t="shared" ref="G3:G48" si="2">IF(F3&gt;0.4,"Urban","Rural")</f>
         <v>Rural</v>
       </c>
       <c r="H3" s="4">
@@ -4010,7 +4207,7 @@
       </c>
       <c r="G18" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>Urban</v>
+        <v>Rural</v>
       </c>
       <c r="H18" s="13">
         <v>2086</v>
@@ -4663,8 +4860,8 @@
         <v>0.31179297648183135</v>
       </c>
       <c r="G25" s="30" t="str">
-        <f>IF(F25&gt;0.25,"Urban","Rural")</f>
-        <v>Urban</v>
+        <f t="shared" si="2"/>
+        <v>Rural</v>
       </c>
       <c r="H25" s="16">
         <v>25991</v>
@@ -4757,7 +4954,7 @@
         <v>0.23323727394325608</v>
       </c>
       <c r="G26" s="30" t="str">
-        <f t="shared" ref="G26:G48" si="3">IF(F26&gt;0.25,"Urban","Rural")</f>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H26" s="18">
@@ -4851,7 +5048,7 @@
         <v>8.9873029551391787E-2</v>
       </c>
       <c r="G27" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H27" s="18">
@@ -4945,7 +5142,7 @@
         <v>0.14976227925290836</v>
       </c>
       <c r="G28" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H28" s="18">
@@ -5039,7 +5236,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Urban</v>
       </c>
       <c r="H29" s="16">
@@ -5135,7 +5332,7 @@
         <v>0.11207885372501514</v>
       </c>
       <c r="G30" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H30" s="18">
@@ -5232,7 +5429,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Urban</v>
       </c>
       <c r="H31" s="19">
@@ -5330,7 +5527,7 @@
         <v>0.48426557740673626</v>
       </c>
       <c r="G32" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Urban</v>
       </c>
       <c r="H32" s="19">
@@ -5427,7 +5624,7 @@
         <v>6.7153958796943927E-2</v>
       </c>
       <c r="G33" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H33" s="19">
@@ -5523,7 +5720,7 @@
         <v>8.6669263382080766E-2</v>
       </c>
       <c r="G34" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H34" s="19">
@@ -5619,7 +5816,7 @@
         <v>7.7671506136306592E-2</v>
       </c>
       <c r="G35" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H35" s="17">
@@ -5716,7 +5913,7 @@
         <v>0.10423961559732348</v>
       </c>
       <c r="G36" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H36" s="19">
@@ -5813,7 +6010,7 @@
         <v>0.19858028041371825</v>
       </c>
       <c r="G37" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H37" s="19">
@@ -5910,7 +6107,7 @@
         <v>0.15187850235396855</v>
       </c>
       <c r="G38" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H38" s="7">
@@ -6004,7 +6201,7 @@
         <v>8.6003284389684478E-2</v>
       </c>
       <c r="G39" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H39" s="4">
@@ -6098,8 +6295,8 @@
         <v>0.27526264343017165</v>
       </c>
       <c r="G40" s="30" t="str">
-        <f t="shared" si="3"/>
-        <v>Urban</v>
+        <f t="shared" si="2"/>
+        <v>Rural</v>
       </c>
       <c r="H40" s="11">
         <v>17084</v>
@@ -6192,7 +6389,7 @@
         <v>0.23966981385882896</v>
       </c>
       <c r="G41" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H41" s="8">
@@ -6286,7 +6483,7 @@
         <v>8.3278014736365549E-2</v>
       </c>
       <c r="G42" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H42" s="23">
@@ -6380,7 +6577,7 @@
         <v>0.18047722956032317</v>
       </c>
       <c r="G43" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H43" s="23">
@@ -6474,7 +6671,7 @@
         <v>0.15188203362330849</v>
       </c>
       <c r="G44" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H44" s="23">
@@ -6568,7 +6765,7 @@
         <v>0.43862718430242453</v>
       </c>
       <c r="G45" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Urban</v>
       </c>
       <c r="H45" s="23">
@@ -6662,7 +6859,7 @@
         <v>9.8953751866484294E-2</v>
       </c>
       <c r="G46" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H46" s="23">
@@ -6756,7 +6953,7 @@
         <v>0.22677894639833193</v>
       </c>
       <c r="G47" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H47" s="23">
@@ -6850,7 +7047,7 @@
         <v>7.410786524590729E-2</v>
       </c>
       <c r="G48" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Rural</v>
       </c>
       <c r="H48" s="11">
@@ -35488,14 +35685,14 @@
   <customSheetViews>
     <customSheetView guid="{94835D04-D966-4448-B29D-63E064533BCB}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:Z48" xr:uid="{2EDD5FAC-8DDA-4C87-B33C-CF81ABBC351A}"/>
+      <autoFilter ref="A1:Z48" xr:uid="{51161E49-7000-4230-88E5-572E29CDB4D6}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -35506,7 +35703,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -35514,7 +35711,7 @@
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="13.2">
       <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
@@ -42513,4 +42710,625 @@
   <autoFilter ref="A1:E236" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9F0FFC-CADE-42C6-A4AE-354992C2BE70}">
+  <dimension ref="A3:D52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4">
+      <c r="A3" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="34">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="34">
+        <v>1</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="34">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="34">
+        <v>1</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="34">
+        <v>1</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="34">
+        <v>1</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="34">
+        <v>1</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="34">
+        <v>1</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34">
+        <v>1</v>
+      </c>
+      <c r="D13" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34">
+        <v>1</v>
+      </c>
+      <c r="D14" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="34">
+        <v>1</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="34">
+        <v>1</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34">
+        <v>1</v>
+      </c>
+      <c r="D17" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="34">
+        <v>1</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="34">
+        <v>1</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="34">
+        <v>1</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="34">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="34">
+        <v>1</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="34">
+        <v>1</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="34">
+        <v>1</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="34">
+        <v>1</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="34">
+        <v>1</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="34">
+        <v>1</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="34">
+        <v>1</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="34">
+        <v>1</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="34">
+        <v>1</v>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="34">
+        <v>1</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34">
+        <v>1</v>
+      </c>
+      <c r="D32" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="34">
+        <v>1</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34">
+        <v>1</v>
+      </c>
+      <c r="D35" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="34">
+        <v>1</v>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="34">
+        <v>1</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="34">
+        <v>1</v>
+      </c>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="34">
+        <v>1</v>
+      </c>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="34">
+        <v>1</v>
+      </c>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="34">
+        <v>1</v>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="34">
+        <v>1</v>
+      </c>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="34">
+        <v>1</v>
+      </c>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="34">
+        <v>1</v>
+      </c>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="34">
+        <v>1</v>
+      </c>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="34">
+        <v>1</v>
+      </c>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="34">
+        <v>1</v>
+      </c>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34">
+        <v>1</v>
+      </c>
+      <c r="D48" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="34">
+        <v>1</v>
+      </c>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="34">
+        <v>1</v>
+      </c>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="34">
+        <v>1</v>
+      </c>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="34">
+        <v>40</v>
+      </c>
+      <c r="C52" s="34">
+        <v>7</v>
+      </c>
+      <c r="D52" s="34">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
document version 2 ready
</commit_message>
<xml_diff>
--- a/Dataset/Dataset.xlsx
+++ b/Dataset/Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aesops\DTE-Datathon\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C137E53-668C-4B2D-830E-50CAD30C8909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CC634F-7097-48CE-B622-CCB615560F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <customWorkbookView name="Filter 1" guid="{94835D04-D966-4448-B29D-63E064533BCB}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -45,10 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="91">
-  <si>
-    <t>Country</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="90">
   <si>
     <t>County</t>
   </si>
@@ -123,9 +120,6 @@
   </si>
   <si>
     <t>population owning mobile phones%</t>
-  </si>
-  <si>
-    <t>Kenya</t>
   </si>
   <si>
     <t>Baringo</t>
@@ -319,6 +313,9 @@
   <si>
     <t>Column Labels</t>
   </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
 </sst>
 </file>
 
@@ -407,7 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -476,7 +473,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2111,7 +2107,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A46ADEC-2704-42EB-813A-FE6DD83CC3BC}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A46ADEC-2704-42EB-813A-FE6DD83CC3BC}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="29">
     <pivotField showAll="0"/>
@@ -2583,10 +2579,10 @@
   <dimension ref="A1:AE1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2605,101 +2601,101 @@
   <sheetData>
     <row r="1" spans="1:31" ht="26.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="AD1" s="2"/>
       <c r="AE1" s="1"/>
     </row>
     <row r="2" spans="1:31" ht="14.4">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4">
         <v>591474</v>
@@ -2792,7 +2788,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4">
         <v>847718</v>
@@ -2882,10 +2878,10 @@
     </row>
     <row r="4" spans="1:31" ht="14.4">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4">
         <v>1480458</v>
@@ -2975,10 +2971,10 @@
     </row>
     <row r="5" spans="1:31" ht="14.4">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4">
         <v>779928</v>
@@ -3068,10 +3064,10 @@
     </row>
     <row r="6" spans="1:31" ht="14.4">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4">
         <v>433901</v>
@@ -3161,10 +3157,10 @@
     </row>
     <row r="7" spans="1:31" ht="14.4">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4">
         <v>532675</v>
@@ -3254,10 +3250,10 @@
     </row>
     <row r="8" spans="1:31" ht="14.4">
       <c r="A8" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" s="7">
         <v>630463</v>
@@ -3348,10 +3344,10 @@
     </row>
     <row r="9" spans="1:31" ht="14.4">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="11">
         <v>1018871</v>
@@ -3441,10 +3437,10 @@
     </row>
     <row r="10" spans="1:31" ht="14.4">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="11">
         <v>142333</v>
@@ -3534,10 +3530,10 @@
     </row>
     <row r="11" spans="1:31" ht="14.4">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="11">
         <v>495218</v>
@@ -3627,10 +3623,10 @@
     </row>
     <row r="12" spans="1:31" ht="14.4">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="8">
         <v>1682239</v>
@@ -3721,10 +3717,10 @@
     </row>
     <row r="13" spans="1:31" ht="14.4">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="11">
         <v>808239</v>
@@ -3813,11 +3809,11 @@
       <c r="AD13" s="5"/>
     </row>
     <row r="14" spans="1:31" ht="14.4">
-      <c r="A14" s="3" t="s">
-        <v>26</v>
+      <c r="A14" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="5">
         <v>711450</v>
@@ -3906,11 +3902,11 @@
       <c r="AD14" s="5"/>
     </row>
     <row r="15" spans="1:31" ht="14.4">
-      <c r="A15" s="3" t="s">
-        <v>26</v>
+      <c r="A15" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5">
         <v>1059899</v>
@@ -3999,11 +3995,11 @@
       <c r="AD15" s="5"/>
     </row>
     <row r="16" spans="1:31" ht="14.4">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
+      <c r="A16" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5">
         <v>474187</v>
@@ -4092,11 +4088,11 @@
       <c r="AD16" s="5"/>
     </row>
     <row r="17" spans="1:31" ht="14.4">
-      <c r="A17" s="3" t="s">
-        <v>26</v>
+      <c r="A17" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5">
         <v>1115450</v>
@@ -4186,10 +4182,10 @@
     </row>
     <row r="18" spans="1:31" ht="14.4">
       <c r="A18" s="12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="13">
         <v>714668</v>
@@ -4279,11 +4275,11 @@
       <c r="AE18" s="14"/>
     </row>
     <row r="19" spans="1:31" ht="14.4">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
+      <c r="A19" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5">
         <v>1082168</v>
@@ -4372,11 +4368,11 @@
       <c r="AD19" s="5"/>
     </row>
     <row r="20" spans="1:31" ht="14.4">
-      <c r="A20" s="3" t="s">
-        <v>26</v>
+      <c r="A20" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5">
         <v>740389</v>
@@ -4465,11 +4461,11 @@
       <c r="AD20" s="5"/>
     </row>
     <row r="21" spans="1:31" ht="14.4">
-      <c r="A21" s="3" t="s">
-        <v>26</v>
+      <c r="A21" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="5">
         <v>391200</v>
@@ -4558,11 +4554,11 @@
       <c r="AD21" s="5"/>
     </row>
     <row r="22" spans="1:31" ht="14.4">
-      <c r="A22" s="3" t="s">
-        <v>26</v>
+      <c r="A22" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="5">
         <v>105474</v>
@@ -4652,10 +4648,10 @@
     </row>
     <row r="23" spans="1:31" ht="14.4">
       <c r="A23" s="6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="9">
         <v>1007854</v>
@@ -4745,11 +4741,11 @@
       <c r="AE23" s="10"/>
     </row>
     <row r="24" spans="1:31" ht="14.4">
-      <c r="A24" s="3" t="s">
-        <v>26</v>
+      <c r="A24" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="16">
         <v>910577</v>
@@ -4839,11 +4835,11 @@
       <c r="AE24" s="17"/>
     </row>
     <row r="25" spans="1:31" ht="14.4">
-      <c r="A25" s="3" t="s">
-        <v>26</v>
+      <c r="A25" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" s="16">
         <v>596990</v>
@@ -4933,11 +4929,11 @@
       <c r="AE25" s="17"/>
     </row>
     <row r="26" spans="1:31" ht="14.4">
-      <c r="A26" s="3" t="s">
-        <v>26</v>
+      <c r="A26" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="18">
         <v>352546</v>
@@ -5027,11 +5023,11 @@
       <c r="AE26" s="17"/>
     </row>
     <row r="27" spans="1:31" ht="14.4">
-      <c r="A27" s="3" t="s">
-        <v>26</v>
+      <c r="A27" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="18">
         <v>1406796</v>
@@ -5121,11 +5117,11 @@
       <c r="AE27" s="17"/>
     </row>
     <row r="28" spans="1:31" ht="14.4">
-      <c r="A28" s="3" t="s">
-        <v>26</v>
+      <c r="A28" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" s="18">
         <v>949236</v>
@@ -5215,11 +5211,11 @@
       <c r="AE28" s="17"/>
     </row>
     <row r="29" spans="1:31" ht="14.4">
-      <c r="A29" s="3" t="s">
-        <v>26</v>
+      <c r="A29" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" s="16">
         <v>0</v>
@@ -5311,11 +5307,11 @@
       <c r="AE29" s="17"/>
     </row>
     <row r="30" spans="1:31" ht="14.4">
-      <c r="A30" s="3" t="s">
-        <v>26</v>
+      <c r="A30" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="18">
         <v>938213</v>
@@ -5408,11 +5404,11 @@
       <c r="AE30" s="17"/>
     </row>
     <row r="31" spans="1:31" ht="14.4">
-      <c r="A31" s="3" t="s">
-        <v>26</v>
+      <c r="A31" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="16">
         <v>0</v>
@@ -5506,11 +5502,11 @@
       <c r="AE31" s="17"/>
     </row>
     <row r="32" spans="1:31" ht="14.4">
-      <c r="A32" s="3" t="s">
-        <v>26</v>
+      <c r="A32" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="19">
         <v>1115122</v>
@@ -5603,11 +5599,11 @@
       <c r="AE32" s="17"/>
     </row>
     <row r="33" spans="1:31" ht="14.4">
-      <c r="A33" s="3" t="s">
-        <v>26</v>
+      <c r="A33" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" s="19">
         <v>826232</v>
@@ -5699,11 +5695,11 @@
       <c r="AE33" s="17"/>
     </row>
     <row r="34" spans="1:31" ht="14.4">
-      <c r="A34" s="3" t="s">
-        <v>26</v>
+      <c r="A34" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C34" s="19">
         <v>1057521</v>
@@ -5795,11 +5791,11 @@
       <c r="AE34" s="17"/>
     </row>
     <row r="35" spans="1:31" ht="14.4">
-      <c r="A35" s="3" t="s">
-        <v>26</v>
+      <c r="A35" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="19">
         <v>558540</v>
@@ -5892,11 +5888,11 @@
       <c r="AE35" s="17"/>
     </row>
     <row r="36" spans="1:31" ht="14.4">
-      <c r="A36" s="3" t="s">
-        <v>26</v>
+      <c r="A36" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="19">
         <v>571754</v>
@@ -5989,11 +5985,11 @@
       <c r="AE36" s="17"/>
     </row>
     <row r="37" spans="1:31" ht="14.4">
-      <c r="A37" s="3" t="s">
-        <v>26</v>
+      <c r="A37" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C37" s="19">
         <v>608409</v>
@@ -6087,10 +6083,10 @@
     </row>
     <row r="38" spans="1:31" ht="14.4">
       <c r="A38" s="6" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C38" s="20">
         <v>263195</v>
@@ -6180,11 +6176,11 @@
       <c r="AE38" s="10"/>
     </row>
     <row r="39" spans="1:31" ht="14.4">
-      <c r="A39" s="3" t="s">
-        <v>26</v>
+      <c r="A39" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" s="22">
         <v>907766</v>
@@ -6274,11 +6270,11 @@
       <c r="AE39" s="24"/>
     </row>
     <row r="40" spans="1:31" ht="14.4">
-      <c r="A40" s="3" t="s">
-        <v>26</v>
+      <c r="A40" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C40" s="11">
         <v>246897</v>
@@ -6369,10 +6365,10 @@
     </row>
     <row r="41" spans="1:31" ht="14.4">
       <c r="A41" s="6" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C41" s="20">
         <v>240221</v>
@@ -6462,11 +6458,11 @@
       <c r="AE41" s="10"/>
     </row>
     <row r="42" spans="1:31" ht="14.4">
-      <c r="A42" s="3" t="s">
-        <v>26</v>
+      <c r="A42" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C42" s="22">
         <v>360434</v>
@@ -6556,11 +6552,11 @@
       <c r="AE42" s="24"/>
     </row>
     <row r="43" spans="1:31" ht="14.4">
-      <c r="A43" s="3" t="s">
-        <v>26</v>
+      <c r="A43" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C43" s="22">
         <v>811607</v>
@@ -6650,11 +6646,11 @@
       <c r="AE43" s="24"/>
     </row>
     <row r="44" spans="1:31" ht="14.4">
-      <c r="A44" s="3" t="s">
-        <v>26</v>
+      <c r="A44" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C44" s="22">
         <v>786185</v>
@@ -6744,11 +6740,11 @@
       <c r="AE44" s="24"/>
     </row>
     <row r="45" spans="1:31" ht="14.4">
-      <c r="A45" s="3" t="s">
-        <v>26</v>
+      <c r="A45" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="22">
         <v>652981</v>
@@ -6838,11 +6834,11 @@
       <c r="AE45" s="24"/>
     </row>
     <row r="46" spans="1:31" ht="14.4">
-      <c r="A46" s="3" t="s">
-        <v>26</v>
+      <c r="A46" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C46" s="22">
         <v>531629</v>
@@ -6932,11 +6928,11 @@
       <c r="AE46" s="24"/>
     </row>
     <row r="47" spans="1:31" ht="14.4">
-      <c r="A47" s="3" t="s">
-        <v>26</v>
+      <c r="A47" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" s="22">
         <v>604089</v>
@@ -7025,12 +7021,12 @@
       <c r="AD47" s="23"/>
       <c r="AE47" s="24"/>
     </row>
-    <row r="48" spans="1:31" ht="14.4">
-      <c r="A48" s="3" t="s">
-        <v>26</v>
+    <row r="48" spans="1:31" ht="13.2">
+      <c r="A48" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C48" s="11">
         <v>107572</v>
@@ -7118,8 +7114,7 @@
       </c>
       <c r="AD48" s="5"/>
     </row>
-    <row r="49" spans="1:30" ht="14.4">
-      <c r="A49" s="3"/>
+    <row r="49" spans="3:30" ht="13.2">
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -7149,8 +7144,7 @@
       <c r="AC49" s="5"/>
       <c r="AD49" s="5"/>
     </row>
-    <row r="50" spans="1:30" ht="14.4">
-      <c r="A50" s="3"/>
+    <row r="50" spans="3:30" ht="13.2">
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -7180,8 +7174,7 @@
       <c r="AC50" s="5"/>
       <c r="AD50" s="5"/>
     </row>
-    <row r="51" spans="1:30" ht="14.4">
-      <c r="A51" s="3"/>
+    <row r="51" spans="3:30" ht="13.2">
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -7211,7 +7204,7 @@
       <c r="AC51" s="5"/>
       <c r="AD51" s="5"/>
     </row>
-    <row r="52" spans="1:30" ht="13.2">
+    <row r="52" spans="3:30" ht="13.2">
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -7241,7 +7234,7 @@
       <c r="AC52" s="5"/>
       <c r="AD52" s="5"/>
     </row>
-    <row r="53" spans="1:30" ht="13.2">
+    <row r="53" spans="3:30" ht="13.2">
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -7271,7 +7264,7 @@
       <c r="AC53" s="5"/>
       <c r="AD53" s="5"/>
     </row>
-    <row r="54" spans="1:30" ht="13.2">
+    <row r="54" spans="3:30" ht="13.2">
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
@@ -7301,7 +7294,7 @@
       <c r="AC54" s="5"/>
       <c r="AD54" s="5"/>
     </row>
-    <row r="55" spans="1:30" ht="13.2">
+    <row r="55" spans="3:30" ht="13.2">
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -7331,7 +7324,7 @@
       <c r="AC55" s="5"/>
       <c r="AD55" s="5"/>
     </row>
-    <row r="56" spans="1:30" ht="13.2">
+    <row r="56" spans="3:30" ht="13.2">
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -7361,7 +7354,7 @@
       <c r="AC56" s="5"/>
       <c r="AD56" s="5"/>
     </row>
-    <row r="57" spans="1:30" ht="13.2">
+    <row r="57" spans="3:30" ht="13.2">
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -7391,7 +7384,7 @@
       <c r="AC57" s="5"/>
       <c r="AD57" s="5"/>
     </row>
-    <row r="58" spans="1:30" ht="13.2">
+    <row r="58" spans="3:30" ht="13.2">
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -7421,7 +7414,7 @@
       <c r="AC58" s="5"/>
       <c r="AD58" s="5"/>
     </row>
-    <row r="59" spans="1:30" ht="13.2">
+    <row r="59" spans="3:30" ht="13.2">
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -7451,7 +7444,7 @@
       <c r="AC59" s="5"/>
       <c r="AD59" s="5"/>
     </row>
-    <row r="60" spans="1:30" ht="13.2">
+    <row r="60" spans="3:30" ht="13.2">
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
@@ -7481,7 +7474,7 @@
       <c r="AC60" s="5"/>
       <c r="AD60" s="5"/>
     </row>
-    <row r="61" spans="1:30" ht="13.2">
+    <row r="61" spans="3:30" ht="13.2">
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -7511,7 +7504,7 @@
       <c r="AC61" s="5"/>
       <c r="AD61" s="5"/>
     </row>
-    <row r="62" spans="1:30" ht="13.2">
+    <row r="62" spans="3:30" ht="13.2">
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -7541,7 +7534,7 @@
       <c r="AC62" s="5"/>
       <c r="AD62" s="5"/>
     </row>
-    <row r="63" spans="1:30" ht="13.2">
+    <row r="63" spans="3:30" ht="13.2">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -7571,7 +7564,7 @@
       <c r="AC63" s="5"/>
       <c r="AD63" s="5"/>
     </row>
-    <row r="64" spans="1:30" ht="13.2">
+    <row r="64" spans="3:30" ht="13.2">
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -35685,7 +35678,7 @@
   <customSheetViews>
     <customSheetView guid="{94835D04-D966-4448-B29D-63E064533BCB}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:Z48" xr:uid="{51161E49-7000-4230-88E5-572E29CDB4D6}"/>
+      <autoFilter ref="A1:Z48" xr:uid="{86904C37-839F-43E4-B2E3-B5483305D742}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35713,27 +35706,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.2">
       <c r="A1" s="25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="E1" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" s="11">
         <v>56570</v>
@@ -35748,7 +35741,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="28">
         <v>45091</v>
@@ -35766,10 +35759,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="11">
         <v>119730</v>
@@ -35784,10 +35777,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="11">
         <v>48827</v>
@@ -35802,10 +35795,10 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="11">
         <v>17461</v>
@@ -35820,10 +35813,10 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="11">
         <v>66124</v>
@@ -35838,7 +35831,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="28">
         <v>45091</v>
@@ -35856,10 +35849,10 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="11">
         <v>171935</v>
@@ -35874,10 +35867,10 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" s="11">
         <v>66220</v>
@@ -35892,10 +35885,10 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C11" s="11">
         <v>23061</v>
@@ -35910,10 +35903,10 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="11">
         <v>134859</v>
@@ -35928,7 +35921,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="28">
         <v>45091</v>
@@ -35946,10 +35939,10 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="25">
         <v>306271</v>
@@ -35964,10 +35957,10 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="25">
         <v>135035</v>
@@ -35982,10 +35975,10 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="25">
         <v>46606</v>
@@ -36000,10 +35993,10 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" s="25">
         <v>69112</v>
@@ -36018,7 +36011,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="28">
         <v>45091</v>
@@ -36036,10 +36029,10 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="25">
         <v>169276</v>
@@ -36054,10 +36047,10 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C20" s="25">
         <v>76898</v>
@@ -36072,10 +36065,10 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" s="25">
         <v>29670</v>
@@ -36090,10 +36083,10 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22" s="25">
         <v>36826</v>
@@ -36108,7 +36101,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" s="28">
         <v>45091</v>
@@ -36126,10 +36119,10 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="25">
         <v>83616</v>
@@ -36144,10 +36137,10 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" s="25">
         <v>35274</v>
@@ -36162,10 +36155,10 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" s="25">
         <v>13350</v>
@@ -36180,10 +36173,10 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C27" s="25">
         <v>36154</v>
@@ -36198,7 +36191,7 @@
     </row>
     <row r="28" spans="1:5" ht="14.4">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="28">
         <v>45091</v>
@@ -36216,10 +36209,10 @@
     </row>
     <row r="29" spans="1:5" ht="14.4">
       <c r="A29" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" s="25">
         <v>107827</v>
@@ -36234,10 +36227,10 @@
     </row>
     <row r="30" spans="1:5" ht="14.4">
       <c r="A30" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30" s="25">
         <v>74576</v>
@@ -36252,10 +36245,10 @@
     </row>
     <row r="31" spans="1:5" ht="14.4">
       <c r="A31" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="25">
         <v>27773</v>
@@ -36270,10 +36263,10 @@
     </row>
     <row r="32" spans="1:5" ht="14.4">
       <c r="A32" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="25">
         <v>67467</v>
@@ -36288,7 +36281,7 @@
     </row>
     <row r="33" spans="1:5" ht="14.4">
       <c r="A33" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" s="28">
         <v>45091</v>
@@ -36306,10 +36299,10 @@
     </row>
     <row r="34" spans="1:5" ht="14.4">
       <c r="A34" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" s="25">
         <v>149908</v>
@@ -36324,10 +36317,10 @@
     </row>
     <row r="35" spans="1:5" ht="14.4">
       <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="25">
         <v>47954</v>
@@ -36342,10 +36335,10 @@
     </row>
     <row r="36" spans="1:5" ht="14.4">
       <c r="A36" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" s="25">
         <v>7773</v>
@@ -36360,10 +36353,10 @@
     </row>
     <row r="37" spans="1:5" ht="14.4">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="25">
         <v>106718</v>
@@ -36378,7 +36371,7 @@
     </row>
     <row r="38" spans="1:5" ht="14.4">
       <c r="A38" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B38" s="28">
         <v>45091</v>
@@ -36396,10 +36389,10 @@
     </row>
     <row r="39" spans="1:5" ht="14.4">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" s="25">
         <v>240582</v>
@@ -36414,10 +36407,10 @@
     </row>
     <row r="40" spans="1:5" ht="14.4">
       <c r="A40" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" s="25">
         <v>82128</v>
@@ -36432,10 +36425,10 @@
     </row>
     <row r="41" spans="1:5" ht="14.4">
       <c r="A41" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="25">
         <v>42637</v>
@@ -36450,10 +36443,10 @@
     </row>
     <row r="42" spans="1:5" ht="14.4">
       <c r="A42" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" s="25">
         <v>24490</v>
@@ -36468,7 +36461,7 @@
     </row>
     <row r="43" spans="1:5" ht="14.4">
       <c r="A43" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B43" s="28">
         <v>45091</v>
@@ -36486,10 +36479,10 @@
     </row>
     <row r="44" spans="1:5" ht="14.4">
       <c r="A44" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C44" s="25">
         <v>47754</v>
@@ -36504,10 +36497,10 @@
     </row>
     <row r="45" spans="1:5" ht="14.4">
       <c r="A45" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" s="25">
         <v>16937</v>
@@ -36522,10 +36515,10 @@
     </row>
     <row r="46" spans="1:5" ht="14.4">
       <c r="A46" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C46" s="25">
         <v>5119</v>
@@ -36540,10 +36533,10 @@
     </row>
     <row r="47" spans="1:5" ht="14.4">
       <c r="A47" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C47" s="25">
         <v>92772</v>
@@ -36558,7 +36551,7 @@
     </row>
     <row r="48" spans="1:5" ht="14.4">
       <c r="A48" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B48" s="28">
         <v>45091</v>
@@ -36576,10 +36569,10 @@
     </row>
     <row r="49" spans="1:5" ht="14.4">
       <c r="A49" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C49" s="25">
         <v>236260</v>
@@ -36594,10 +36587,10 @@
     </row>
     <row r="50" spans="1:5" ht="14.4">
       <c r="A50" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C50" s="25">
         <v>92064</v>
@@ -36612,10 +36605,10 @@
     </row>
     <row r="51" spans="1:5" ht="14.4">
       <c r="A51" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C51" s="25">
         <v>16976</v>
@@ -36630,10 +36623,10 @@
     </row>
     <row r="52" spans="1:5" ht="14.4">
       <c r="A52" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C52" s="25">
         <v>138917</v>
@@ -36648,7 +36641,7 @@
     </row>
     <row r="53" spans="1:5" ht="14.4">
       <c r="A53" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B53" s="28">
         <v>45091</v>
@@ -36666,10 +36659,10 @@
     </row>
     <row r="54" spans="1:5" ht="14.4">
       <c r="A54" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C54" s="25">
         <v>339313</v>
@@ -36684,10 +36677,10 @@
     </row>
     <row r="55" spans="1:5" ht="14.4">
       <c r="A55" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C55" s="25">
         <v>170612</v>
@@ -36702,10 +36695,10 @@
     </row>
     <row r="56" spans="1:5" ht="14.4">
       <c r="A56" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C56" s="25">
         <v>65350</v>
@@ -36720,10 +36713,10 @@
     </row>
     <row r="57" spans="1:5" ht="14.4">
       <c r="A57" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C57" s="25">
         <v>65733</v>
@@ -36738,7 +36731,7 @@
     </row>
     <row r="58" spans="1:5" ht="14.4">
       <c r="A58" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B58" s="28">
         <v>45091</v>
@@ -36756,10 +36749,10 @@
     </row>
     <row r="59" spans="1:5" ht="14.4">
       <c r="A59" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C59" s="25">
         <v>179018</v>
@@ -36774,10 +36767,10 @@
     </row>
     <row r="60" spans="1:5" ht="14.4">
       <c r="A60" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C60" s="25">
         <v>72828</v>
@@ -36792,10 +36785,10 @@
     </row>
     <row r="61" spans="1:5" ht="14.4">
       <c r="A61" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C61" s="25">
         <v>23087</v>
@@ -36810,10 +36803,10 @@
     </row>
     <row r="62" spans="1:5" ht="14.4">
       <c r="A62" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C62" s="25">
         <v>162238</v>
@@ -36828,7 +36821,7 @@
     </row>
     <row r="63" spans="1:5" ht="14.4">
       <c r="A63" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B63" s="28">
         <v>45091</v>
@@ -36846,10 +36839,10 @@
     </row>
     <row r="64" spans="1:5" ht="14.4">
       <c r="A64" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C64" s="25">
         <v>527002</v>
@@ -36864,10 +36857,10 @@
     </row>
     <row r="65" spans="1:5" ht="14.4">
       <c r="A65" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C65" s="25">
         <v>267888</v>
@@ -36882,10 +36875,10 @@
     </row>
     <row r="66" spans="1:5" ht="14.4">
       <c r="A66" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C66" s="25">
         <v>62605</v>
@@ -36900,10 +36893,10 @@
     </row>
     <row r="67" spans="1:5" ht="14.4">
       <c r="A67" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C67" s="25">
         <v>121527</v>
@@ -36918,7 +36911,7 @@
     </row>
     <row r="68" spans="1:5" ht="14.4">
       <c r="A68" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B68" s="28">
         <v>45091</v>
@@ -36936,10 +36929,10 @@
     </row>
     <row r="69" spans="1:5" ht="14.4">
       <c r="A69" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C69" s="25">
         <v>281638</v>
@@ -36954,10 +36947,10 @@
     </row>
     <row r="70" spans="1:5" ht="14.4">
       <c r="A70" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C70" s="25">
         <v>118135</v>
@@ -36972,10 +36965,10 @@
     </row>
     <row r="71" spans="1:5" ht="14.4">
       <c r="A71" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C71" s="25">
         <v>44326</v>
@@ -36990,10 +36983,10 @@
     </row>
     <row r="72" spans="1:5" ht="14.4">
       <c r="A72" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C72" s="25">
         <v>34082</v>
@@ -37008,7 +37001,7 @@
     </row>
     <row r="73" spans="1:5" ht="14.4">
       <c r="A73" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B73" s="28">
         <v>45091</v>
@@ -37026,10 +37019,10 @@
     </row>
     <row r="74" spans="1:5" ht="14.4">
       <c r="A74" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C74" s="25">
         <v>105255</v>
@@ -37044,10 +37037,10 @@
     </row>
     <row r="75" spans="1:5" ht="14.4">
       <c r="A75" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C75" s="25">
         <v>86888</v>
@@ -37062,10 +37055,10 @@
     </row>
     <row r="76" spans="1:5" ht="14.4">
       <c r="A76" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C76" s="25">
         <v>28635</v>
@@ -37080,10 +37073,10 @@
     </row>
     <row r="77" spans="1:5" ht="14.4">
       <c r="A77" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C77" s="25">
         <v>87507</v>
@@ -37098,7 +37091,7 @@
     </row>
     <row r="78" spans="1:5" ht="14.4">
       <c r="A78" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B78" s="28">
         <v>45091</v>
@@ -37116,10 +37109,10 @@
     </row>
     <row r="79" spans="1:5" ht="14.4">
       <c r="A79" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C79" s="25">
         <v>247941</v>
@@ -37134,10 +37127,10 @@
     </row>
     <row r="80" spans="1:5" ht="14.4">
       <c r="A80" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C80" s="25">
         <v>114486</v>
@@ -37152,10 +37145,10 @@
     </row>
     <row r="81" spans="1:5" ht="14.4">
       <c r="A81" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C81" s="25">
         <v>43721</v>
@@ -37170,10 +37163,10 @@
     </row>
     <row r="82" spans="1:5" ht="14.4">
       <c r="A82" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C82" s="25">
         <v>84902</v>
@@ -37188,7 +37181,7 @@
     </row>
     <row r="83" spans="1:5" ht="14.4">
       <c r="A83" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B83" s="28">
         <v>45091</v>
@@ -37206,10 +37199,10 @@
     </row>
     <row r="84" spans="1:5" ht="14.4">
       <c r="A84" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C84" s="25">
         <v>240025</v>
@@ -37224,10 +37217,10 @@
     </row>
     <row r="85" spans="1:5" ht="14.4">
       <c r="A85" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C85" s="25">
         <v>92885</v>
@@ -37242,10 +37235,10 @@
     </row>
     <row r="86" spans="1:5" ht="14.4">
       <c r="A86" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C86" s="25">
         <v>34176</v>
@@ -37260,10 +37253,10 @@
     </row>
     <row r="87" spans="1:5" ht="14.4">
       <c r="A87" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C87" s="25">
         <v>76426</v>
@@ -37278,7 +37271,7 @@
     </row>
     <row r="88" spans="1:5" ht="14.4">
       <c r="A88" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B88" s="28">
         <v>45091</v>
@@ -37296,10 +37289,10 @@
     </row>
     <row r="89" spans="1:5" ht="14.4">
       <c r="A89" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C89" s="25">
         <v>202518</v>
@@ -37314,10 +37307,10 @@
     </row>
     <row r="90" spans="1:5" ht="14.4">
       <c r="A90" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C90" s="25">
         <v>113421</v>
@@ -37332,10 +37325,10 @@
     </row>
     <row r="91" spans="1:5" ht="14.4">
       <c r="A91" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C91" s="25">
         <v>51401</v>
@@ -37350,10 +37343,10 @@
     </row>
     <row r="92" spans="1:5" ht="14.4">
       <c r="A92" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C92" s="25">
         <v>78851</v>
@@ -37368,7 +37361,7 @@
     </row>
     <row r="93" spans="1:5" ht="14.4">
       <c r="A93" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B93" s="28">
         <v>45091</v>
@@ -37386,10 +37379,10 @@
     </row>
     <row r="94" spans="1:5" ht="14.4">
       <c r="A94" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C94" s="25">
         <v>158195</v>
@@ -37404,10 +37397,10 @@
     </row>
     <row r="95" spans="1:5" ht="14.4">
       <c r="A95" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C95" s="25">
         <v>67911</v>
@@ -37422,10 +37415,10 @@
     </row>
     <row r="96" spans="1:5" ht="14.4">
       <c r="A96" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C96" s="25">
         <v>23674</v>
@@ -37440,10 +37433,10 @@
     </row>
     <row r="97" spans="1:5" ht="14.4">
       <c r="A97" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C97" s="25">
         <v>38806</v>
@@ -37458,7 +37451,7 @@
     </row>
     <row r="98" spans="1:5" ht="14.4">
       <c r="A98" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B98" s="28">
         <v>45091</v>
@@ -37476,10 +37469,10 @@
     </row>
     <row r="99" spans="1:5" ht="14.4">
       <c r="A99" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C99" s="25">
         <v>92491</v>
@@ -37494,10 +37487,10 @@
     </row>
     <row r="100" spans="1:5" ht="14.4">
       <c r="A100" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C100" s="25">
         <v>53185</v>
@@ -37512,10 +37505,10 @@
     </row>
     <row r="101" spans="1:5" ht="14.4">
       <c r="A101" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C101" s="25">
         <v>17300</v>
@@ -37530,10 +37523,10 @@
     </row>
     <row r="102" spans="1:5" ht="14.4">
       <c r="A102" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C102" s="25">
         <v>11042</v>
@@ -37548,7 +37541,7 @@
     </row>
     <row r="103" spans="1:5" ht="14.4">
       <c r="A103" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B103" s="28">
         <v>45091</v>
@@ -37566,10 +37559,10 @@
     </row>
     <row r="104" spans="1:5" ht="14.4">
       <c r="A104" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C104" s="25">
         <v>24247</v>
@@ -37584,10 +37577,10 @@
     </row>
     <row r="105" spans="1:5" ht="14.4">
       <c r="A105" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C105" s="25">
         <v>12455</v>
@@ -37602,10 +37595,10 @@
     </row>
     <row r="106" spans="1:5" ht="14.4">
       <c r="A106" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C106" s="25">
         <v>3754</v>
@@ -37620,10 +37613,10 @@
     </row>
     <row r="107" spans="1:5" ht="14.4">
       <c r="A107" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C107" s="25">
         <v>87157</v>
@@ -37638,7 +37631,7 @@
     </row>
     <row r="108" spans="1:5" ht="14.4">
       <c r="A108" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B108" s="28">
         <v>45091</v>
@@ -37656,10 +37649,10 @@
     </row>
     <row r="109" spans="1:5" ht="14.4">
       <c r="A109" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C109" s="25">
         <v>266331</v>
@@ -37674,10 +37667,10 @@
     </row>
     <row r="110" spans="1:5" ht="14.4">
       <c r="A110" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C110" s="25">
         <v>156292</v>
@@ -37692,10 +37685,10 @@
     </row>
     <row r="111" spans="1:5" ht="14.4">
       <c r="A111" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C111" s="25">
         <v>59569</v>
@@ -37710,10 +37703,10 @@
     </row>
     <row r="112" spans="1:5" ht="14.4">
       <c r="A112" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C112" s="25">
         <v>58018</v>
@@ -37728,7 +37721,7 @@
     </row>
     <row r="113" spans="1:5" ht="14.4">
       <c r="A113" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B113" s="28">
         <v>45091</v>
@@ -37746,10 +37739,10 @@
     </row>
     <row r="114" spans="1:5" ht="14.4">
       <c r="A114" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C114" s="25">
         <v>172667</v>
@@ -37764,10 +37757,10 @@
     </row>
     <row r="115" spans="1:5" ht="14.4">
       <c r="A115" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C115" s="25">
         <v>106120</v>
@@ -37782,10 +37775,10 @@
     </row>
     <row r="116" spans="1:5" ht="14.4">
       <c r="A116" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C116" s="25">
         <v>49167</v>
@@ -37800,10 +37793,10 @@
     </row>
     <row r="117" spans="1:5" ht="14.4">
       <c r="A117" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C117" s="25">
         <v>102319</v>
@@ -37818,7 +37811,7 @@
     </row>
     <row r="118" spans="1:5" ht="14.4">
       <c r="A118" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B118" s="28">
         <v>45091</v>
@@ -37836,10 +37829,10 @@
     </row>
     <row r="119" spans="1:5" ht="14.4">
       <c r="A119" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C119" s="25">
         <v>142663</v>
@@ -37854,10 +37847,10 @@
     </row>
     <row r="120" spans="1:5" ht="14.4">
       <c r="A120" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C120" s="25">
         <v>38986</v>
@@ -37872,10 +37865,10 @@
     </row>
     <row r="121" spans="1:5" ht="14.4">
       <c r="A121" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C121" s="25">
         <v>6811</v>
@@ -37890,10 +37883,10 @@
     </row>
     <row r="122" spans="1:5" ht="14.4">
       <c r="A122" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C122" s="11">
         <v>41669</v>
@@ -37908,7 +37901,7 @@
     </row>
     <row r="123" spans="1:5" ht="14.4">
       <c r="A123" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B123" s="28">
         <v>45091</v>
@@ -37926,10 +37919,10 @@
     </row>
     <row r="124" spans="1:5" ht="14.4">
       <c r="A124" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C124" s="11">
         <v>77174</v>
@@ -37944,10 +37937,10 @@
     </row>
     <row r="125" spans="1:5" ht="14.4">
       <c r="A125" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C125" s="11">
         <v>26338</v>
@@ -37962,10 +37955,10 @@
     </row>
     <row r="126" spans="1:5" ht="14.4">
       <c r="A126" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C126" s="11">
         <v>8278</v>
@@ -37980,10 +37973,10 @@
     </row>
     <row r="127" spans="1:5" ht="14.4">
       <c r="A127" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C127" s="11">
         <v>101724</v>
@@ -37998,7 +37991,7 @@
     </row>
     <row r="128" spans="1:5" ht="14.4">
       <c r="A128" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B128" s="28">
         <v>45091</v>
@@ -38016,10 +38009,10 @@
     </row>
     <row r="129" spans="1:5" ht="14.4">
       <c r="A129" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C129" s="11">
         <v>284097</v>
@@ -38034,10 +38027,10 @@
     </row>
     <row r="130" spans="1:5" ht="14.4">
       <c r="A130" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C130" s="11">
         <v>164557</v>
@@ -38052,10 +38045,10 @@
     </row>
     <row r="131" spans="1:5" ht="14.4">
       <c r="A131" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C131" s="11">
         <v>60281</v>
@@ -38070,10 +38063,10 @@
     </row>
     <row r="132" spans="1:5" ht="14.4">
       <c r="A132" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C132" s="11">
         <v>98902</v>
@@ -38088,7 +38081,7 @@
     </row>
     <row r="133" spans="1:5" ht="14.4">
       <c r="A133" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B133" s="28">
         <v>45091</v>
@@ -38106,10 +38099,10 @@
     </row>
     <row r="134" spans="1:5" ht="14.4">
       <c r="A134" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C134" s="11">
         <v>215232</v>
@@ -38124,10 +38117,10 @@
     </row>
     <row r="135" spans="1:5" ht="14.4">
       <c r="A135" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C135" s="11">
         <v>79267</v>
@@ -38142,10 +38135,10 @@
     </row>
     <row r="136" spans="1:5" ht="14.4">
       <c r="A136" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C136" s="11">
         <v>27945</v>
@@ -38160,10 +38153,10 @@
     </row>
     <row r="137" spans="1:5" ht="14.4">
       <c r="A137" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C137" s="11">
         <v>87201</v>
@@ -38178,7 +38171,7 @@
     </row>
     <row r="138" spans="1:5" ht="14.4">
       <c r="A138" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B138" s="28">
         <v>45091</v>
@@ -38196,10 +38189,10 @@
     </row>
     <row r="139" spans="1:5" ht="14.4">
       <c r="A139" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C139" s="11">
         <v>274161</v>
@@ -38214,10 +38207,10 @@
     </row>
     <row r="140" spans="1:5" ht="14.4">
       <c r="A140" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C140" s="11">
         <v>110120</v>
@@ -38232,10 +38225,10 @@
     </row>
     <row r="141" spans="1:5" ht="14.4">
       <c r="A141" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C141" s="11">
         <v>16836</v>
@@ -38250,10 +38243,10 @@
     </row>
     <row r="142" spans="1:5" ht="14.4">
       <c r="A142" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C142" s="11">
         <v>65653</v>
@@ -38268,7 +38261,7 @@
     </row>
     <row r="143" spans="1:5" ht="14.4">
       <c r="A143" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B143" s="28">
         <v>45091</v>
@@ -38286,10 +38279,10 @@
     </row>
     <row r="144" spans="1:5" ht="14.4">
       <c r="A144" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C144" s="11">
         <v>165268</v>
@@ -38304,10 +38297,10 @@
     </row>
     <row r="145" spans="1:5" ht="14.4">
       <c r="A145" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C145" s="11">
         <v>135361</v>
@@ -38322,10 +38315,10 @@
     </row>
     <row r="146" spans="1:5" ht="14.4">
       <c r="A146" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C146" s="11">
         <v>62721</v>
@@ -38340,10 +38333,10 @@
     </row>
     <row r="147" spans="1:5" ht="14.4">
       <c r="A147" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C147" s="11">
         <v>305599</v>
@@ -38358,7 +38351,7 @@
     </row>
     <row r="148" spans="1:5" ht="14.4">
       <c r="A148" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B148" s="28">
         <v>45091</v>
@@ -38376,10 +38369,10 @@
     </row>
     <row r="149" spans="1:5" ht="14.4">
       <c r="A149" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C149" s="11">
         <v>1097131</v>
@@ -38394,10 +38387,10 @@
     </row>
     <row r="150" spans="1:5" ht="14.4">
       <c r="A150" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C150" s="11">
         <v>393782</v>
@@ -38412,10 +38405,10 @@
     </row>
     <row r="151" spans="1:5" ht="14.4">
       <c r="A151" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C151" s="11">
         <v>41482</v>
@@ -38430,10 +38423,10 @@
     </row>
     <row r="152" spans="1:5" ht="14.4">
       <c r="A152" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C152" s="25">
         <v>161243</v>
@@ -38448,7 +38441,7 @@
     </row>
     <row r="153" spans="1:5" ht="14.4">
       <c r="A153" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B153" s="28">
         <v>45091</v>
@@ -38466,10 +38459,10 @@
     </row>
     <row r="154" spans="1:5" ht="14.4">
       <c r="A154" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C154" s="25">
         <v>427854</v>
@@ -38484,10 +38477,10 @@
     </row>
     <row r="155" spans="1:5" ht="14.4">
       <c r="A155" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C155" s="25">
         <v>201557</v>
@@ -38502,10 +38495,10 @@
     </row>
     <row r="156" spans="1:5" ht="14.4">
       <c r="A156" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C156" s="25">
         <v>51639</v>
@@ -38520,10 +38513,10 @@
     </row>
     <row r="157" spans="1:5" ht="14.4">
       <c r="A157" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C157" s="25">
         <v>63563</v>
@@ -38538,7 +38531,7 @@
     </row>
     <row r="158" spans="1:5" ht="14.4">
       <c r="A158" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B158" s="28">
         <v>45091</v>
@@ -38556,10 +38549,10 @@
     </row>
     <row r="159" spans="1:5" ht="14.4">
       <c r="A159" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C159" s="25">
         <v>170267</v>
@@ -38574,10 +38567,10 @@
     </row>
     <row r="160" spans="1:5" ht="14.4">
       <c r="A160" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C160" s="25">
         <v>76404</v>
@@ -38592,10 +38585,10 @@
     </row>
     <row r="161" spans="1:5" ht="14.4">
       <c r="A161" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C161" s="25">
         <v>25065</v>
@@ -38610,10 +38603,10 @@
     </row>
     <row r="162" spans="1:5" ht="14.4">
       <c r="A162" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C162" s="11">
         <v>114048</v>
@@ -38628,7 +38621,7 @@
     </row>
     <row r="163" spans="1:5" ht="14.4">
       <c r="A163" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B163" s="28">
         <v>45091</v>
@@ -38646,10 +38639,10 @@
     </row>
     <row r="164" spans="1:5" ht="14.4">
       <c r="A164" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C164" s="11">
         <v>203801</v>
@@ -38664,10 +38657,10 @@
     </row>
     <row r="165" spans="1:5" ht="14.4">
       <c r="A165" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C165" s="11">
         <v>75585</v>
@@ -38682,10 +38675,10 @@
     </row>
     <row r="166" spans="1:5" ht="14.4">
       <c r="A166" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C166" s="11">
         <v>19050</v>
@@ -38700,10 +38693,10 @@
     </row>
     <row r="167" spans="1:5" ht="14.4">
       <c r="A167" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C167" s="11">
         <v>39518</v>
@@ -38718,7 +38711,7 @@
     </row>
     <row r="168" spans="1:5" ht="14.4">
       <c r="A168" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B168" s="28">
         <v>45091</v>
@@ -38736,10 +38729,10 @@
     </row>
     <row r="169" spans="1:5" ht="14.4">
       <c r="A169" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C169" s="11">
         <v>115601</v>
@@ -38754,10 +38747,10 @@
     </row>
     <row r="170" spans="1:5" ht="14.4">
       <c r="A170" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C170" s="11">
         <v>59229</v>
@@ -38772,10 +38765,10 @@
     </row>
     <row r="171" spans="1:5" ht="14.4">
       <c r="A171" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C171" s="11">
         <v>22146</v>
@@ -38790,10 +38783,10 @@
     </row>
     <row r="172" spans="1:5" ht="14.4">
       <c r="A172" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C172" s="11">
         <v>41534</v>
@@ -38808,7 +38801,7 @@
     </row>
     <row r="173" spans="1:5" ht="14.4">
       <c r="A173" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B173" s="28">
         <v>45091</v>
@@ -38826,10 +38819,10 @@
     </row>
     <row r="174" spans="1:5" ht="14.4">
       <c r="A174" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C174" s="11">
         <v>108240</v>
@@ -38844,10 +38837,10 @@
     </row>
     <row r="175" spans="1:5" ht="14.4">
       <c r="A175" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C175" s="11">
         <v>77650</v>
@@ -38862,10 +38855,10 @@
     </row>
     <row r="176" spans="1:5" ht="14.4">
       <c r="A176" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C176" s="11">
         <v>25451</v>
@@ -38880,10 +38873,10 @@
     </row>
     <row r="177" spans="1:5" ht="14.4">
       <c r="A177" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C177" s="25">
         <v>43282</v>
@@ -38898,7 +38891,7 @@
     </row>
     <row r="178" spans="1:5" ht="14.4">
       <c r="A178" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B178" s="28">
         <v>45091</v>
@@ -38916,10 +38909,10 @@
     </row>
     <row r="179" spans="1:5" ht="14.4">
       <c r="A179" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C179" s="11">
         <v>125082</v>
@@ -38934,10 +38927,10 @@
     </row>
     <row r="180" spans="1:5" ht="14.4">
       <c r="A180" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C180" s="11">
         <v>106632</v>
@@ -38952,10 +38945,10 @@
     </row>
     <row r="181" spans="1:5" ht="14.4">
       <c r="A181" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C181" s="11">
         <v>42252</v>
@@ -38970,10 +38963,10 @@
     </row>
     <row r="182" spans="1:5" ht="14.4">
       <c r="A182" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C182" s="11">
         <v>31034</v>
@@ -38988,7 +38981,7 @@
     </row>
     <row r="183" spans="1:5" ht="14.4">
       <c r="A183" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B183" s="28">
         <v>45091</v>
@@ -39006,10 +38999,10 @@
     </row>
     <row r="184" spans="1:5" ht="14.4">
       <c r="A184" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C184" s="11">
         <v>54464</v>
@@ -39024,10 +39017,10 @@
     </row>
     <row r="185" spans="1:5" ht="14.4">
       <c r="A185" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C185" s="11">
         <v>17924</v>
@@ -39042,10 +39035,10 @@
     </row>
     <row r="186" spans="1:5" ht="14.4">
       <c r="A186" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C186" s="11">
         <v>6490</v>
@@ -39060,10 +39053,10 @@
     </row>
     <row r="187" spans="1:5" ht="14.4">
       <c r="A187" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C187" s="11">
         <v>88900</v>
@@ -39078,7 +39071,7 @@
     </row>
     <row r="188" spans="1:5" ht="14.4">
       <c r="A188" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B188" s="28">
         <v>45091</v>
@@ -39096,10 +39089,10 @@
     </row>
     <row r="189" spans="1:5" ht="14.4">
       <c r="A189" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C189" s="11">
         <v>214097</v>
@@ -39114,10 +39107,10 @@
     </row>
     <row r="190" spans="1:5" ht="14.4">
       <c r="A190" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C190" s="11">
         <v>98433</v>
@@ -39132,10 +39125,10 @@
     </row>
     <row r="191" spans="1:5" ht="14.4">
       <c r="A191" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C191" s="11">
         <v>80715</v>
@@ -39150,10 +39143,10 @@
     </row>
     <row r="192" spans="1:5" ht="14.4">
       <c r="A192" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C192" s="11">
         <v>22989</v>
@@ -39168,7 +39161,7 @@
     </row>
     <row r="193" spans="1:5" ht="14.4">
       <c r="A193" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B193" s="28">
         <v>45091</v>
@@ -39186,10 +39179,10 @@
     </row>
     <row r="194" spans="1:5" ht="14.4">
       <c r="A194" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C194" s="11">
         <v>58660</v>
@@ -39204,10 +39197,10 @@
     </row>
     <row r="195" spans="1:5" ht="14.4">
       <c r="A195" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C195" s="11">
         <v>36892</v>
@@ -39222,10 +39215,10 @@
     </row>
     <row r="196" spans="1:5" ht="14.4">
       <c r="A196" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C196" s="11">
         <v>14182</v>
@@ -39240,10 +39233,10 @@
     </row>
     <row r="197" spans="1:5" ht="14.4">
       <c r="A197" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C197" s="11">
         <v>31530</v>
@@ -39258,7 +39251,7 @@
     </row>
     <row r="198" spans="1:5" ht="14.4">
       <c r="A198" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B198" s="28">
         <v>45091</v>
@@ -39276,10 +39269,10 @@
     </row>
     <row r="199" spans="1:5" ht="14.4">
       <c r="A199" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C199" s="11">
         <v>54019</v>
@@ -39294,10 +39287,10 @@
     </row>
     <row r="200" spans="1:5" ht="14.4">
       <c r="A200" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C200" s="11">
         <v>21824</v>
@@ -39312,10 +39305,10 @@
     </row>
     <row r="201" spans="1:5" ht="14.4">
       <c r="A201" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C201" s="11">
         <v>6692</v>
@@ -39330,10 +39323,10 @@
     </row>
     <row r="202" spans="1:5" ht="14.4">
       <c r="A202" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C202" s="11">
         <v>24355</v>
@@ -39348,7 +39341,7 @@
     </row>
     <row r="203" spans="1:5" ht="14.4">
       <c r="A203" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B203" s="28">
         <v>45091</v>
@@ -39366,10 +39359,10 @@
     </row>
     <row r="204" spans="1:5" ht="14.4">
       <c r="A204" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C204" s="11">
         <v>69172</v>
@@ -39384,10 +39377,10 @@
     </row>
     <row r="205" spans="1:5" ht="14.4">
       <c r="A205" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C205" s="11">
         <v>45013</v>
@@ -39402,10 +39395,10 @@
     </row>
     <row r="206" spans="1:5" ht="14.4">
       <c r="A206" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C206" s="11">
         <v>19629</v>
@@ -39420,10 +39413,10 @@
     </row>
     <row r="207" spans="1:5" ht="14.4">
       <c r="A207" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C207" s="11">
         <v>78043</v>
@@ -39438,7 +39431,7 @@
     </row>
     <row r="208" spans="1:5" ht="14.4">
       <c r="A208" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B208" s="28">
         <v>45091</v>
@@ -39456,10 +39449,10 @@
     </row>
     <row r="209" spans="1:5" ht="14.4">
       <c r="A209" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C209" s="11">
         <v>182497</v>
@@ -39474,10 +39467,10 @@
     </row>
     <row r="210" spans="1:5" ht="14.4">
       <c r="A210" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C210" s="11">
         <v>83702</v>
@@ -39492,10 +39485,10 @@
     </row>
     <row r="211" spans="1:5" ht="14.4">
       <c r="A211" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C211" s="11">
         <v>25293</v>
@@ -39510,10 +39503,10 @@
     </row>
     <row r="212" spans="1:5" ht="14.4">
       <c r="A212" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C212" s="11">
         <v>80848</v>
@@ -39528,7 +39521,7 @@
     </row>
     <row r="213" spans="1:5" ht="14.4">
       <c r="A213" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B213" s="28">
         <v>45091</v>
@@ -39546,10 +39539,10 @@
     </row>
     <row r="214" spans="1:5" ht="14.4">
       <c r="A214" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C214" s="11">
         <v>169172</v>
@@ -39564,10 +39557,10 @@
     </row>
     <row r="215" spans="1:5" ht="14.4">
       <c r="A215" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C215" s="11">
         <v>59181</v>
@@ -39582,10 +39575,10 @@
     </row>
     <row r="216" spans="1:5" ht="14.4">
       <c r="A216" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C216" s="11">
         <v>17004</v>
@@ -39600,10 +39593,10 @@
     </row>
     <row r="217" spans="1:5" ht="14.4">
       <c r="A217" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C217" s="11">
         <v>83138</v>
@@ -39618,7 +39611,7 @@
     </row>
     <row r="218" spans="1:5" ht="14.4">
       <c r="A218" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B218" s="28">
         <v>45091</v>
@@ -39636,10 +39629,10 @@
     </row>
     <row r="219" spans="1:5" ht="14.4">
       <c r="A219" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C219" s="11">
         <v>244368</v>
@@ -39654,10 +39647,10 @@
     </row>
     <row r="220" spans="1:5" ht="14.4">
       <c r="A220" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C220" s="11">
         <v>100807</v>
@@ -39672,10 +39665,10 @@
     </row>
     <row r="221" spans="1:5" ht="14.4">
       <c r="A221" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C221" s="11">
         <v>24690</v>
@@ -39690,10 +39683,10 @@
     </row>
     <row r="222" spans="1:5" ht="14.4">
       <c r="A222" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C222" s="11">
         <v>39526</v>
@@ -39708,7 +39701,7 @@
     </row>
     <row r="223" spans="1:5" ht="14.4">
       <c r="A223" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B223" s="28">
         <v>45091</v>
@@ -39726,10 +39719,10 @@
     </row>
     <row r="224" spans="1:5" ht="14.4">
       <c r="A224" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C224" s="11">
         <v>98668</v>
@@ -39744,10 +39737,10 @@
     </row>
     <row r="225" spans="1:5" ht="14.4">
       <c r="A225" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C225" s="11">
         <v>59701</v>
@@ -39762,10 +39755,10 @@
     </row>
     <row r="226" spans="1:5" ht="14.4">
       <c r="A226" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C226" s="11">
         <v>32133</v>
@@ -39780,10 +39773,10 @@
     </row>
     <row r="227" spans="1:5" ht="14.4">
       <c r="A227" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C227" s="11">
         <v>73695</v>
@@ -39798,7 +39791,7 @@
     </row>
     <row r="228" spans="1:5" ht="14.4">
       <c r="A228" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B228" s="28">
         <v>45091</v>
@@ -39816,10 +39809,10 @@
     </row>
     <row r="229" spans="1:5" ht="14.4">
       <c r="A229" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C229" s="11">
         <v>132577</v>
@@ -39834,10 +39827,10 @@
     </row>
     <row r="230" spans="1:5" ht="14.4">
       <c r="A230" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C230" s="11">
         <v>39818</v>
@@ -39852,10 +39845,10 @@
     </row>
     <row r="231" spans="1:5" ht="14.4">
       <c r="A231" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C231" s="11">
         <v>5932</v>
@@ -39870,10 +39863,10 @@
     </row>
     <row r="232" spans="1:5" ht="13.2">
       <c r="A232" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C232" s="11">
         <v>68078</v>
@@ -39888,7 +39881,7 @@
     </row>
     <row r="233" spans="1:5" ht="13.2">
       <c r="A233" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B233" s="28">
         <v>45091</v>
@@ -39906,10 +39899,10 @@
     </row>
     <row r="234" spans="1:5" ht="13.2">
       <c r="A234" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C234" s="11">
         <v>106588</v>
@@ -39924,10 +39917,10 @@
     </row>
     <row r="235" spans="1:5" ht="13.2">
       <c r="A235" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C235" s="11">
         <v>36407</v>
@@ -39942,10 +39935,10 @@
     </row>
     <row r="236" spans="1:5" ht="13.2">
       <c r="A236" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C236" s="11">
         <v>12840</v>
@@ -42730,601 +42723,554 @@
   <sheetData>
     <row r="3" spans="1:4">
       <c r="A3" s="32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="34">
+        <v>25</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34">
+      <c r="D5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="34">
+        <v>26</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34">
+      <c r="D6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="34">
+        <v>27</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34">
+      <c r="D7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="34">
+        <v>28</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34">
+      <c r="D8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="34">
+        <v>29</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34">
+      <c r="D9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="34">
+        <v>30</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34">
+      <c r="D10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="34">
+        <v>31</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34">
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="34">
+        <v>32</v>
+      </c>
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34">
+      <c r="D12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34">
+        <v>33</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34">
+        <v>34</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="34">
+        <v>35</v>
+      </c>
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34">
+      <c r="D15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="34">
+        <v>36</v>
+      </c>
+      <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34">
+      <c r="D16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34">
+        <v>37</v>
+      </c>
+      <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="34">
+        <v>38</v>
+      </c>
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34">
+      <c r="D18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="34">
+        <v>39</v>
+      </c>
+      <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34">
+      <c r="D19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="34">
+        <v>40</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34">
+      <c r="D20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="34">
+        <v>41</v>
+      </c>
+      <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34">
+      <c r="D21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="34">
+        <v>42</v>
+      </c>
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34">
+      <c r="D22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="34">
+        <v>43</v>
+      </c>
+      <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34">
+      <c r="D23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="34">
+        <v>44</v>
+      </c>
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34">
+      <c r="D24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="34">
+        <v>45</v>
+      </c>
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34">
+      <c r="D25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="34">
+        <v>46</v>
+      </c>
+      <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34">
+      <c r="D26">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="34">
+        <v>47</v>
+      </c>
+      <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34">
+      <c r="D27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="34">
+        <v>48</v>
+      </c>
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34">
+      <c r="D28">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="34">
+        <v>49</v>
+      </c>
+      <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34">
+      <c r="D29">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="34">
+        <v>50</v>
+      </c>
+      <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34">
+      <c r="D30">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="34">
+        <v>51</v>
+      </c>
+      <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34">
+      <c r="D31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34">
+        <v>52</v>
+      </c>
+      <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="34">
+        <v>53</v>
+      </c>
+      <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34">
+      <c r="D33">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34">
+        <v>54</v>
+      </c>
+      <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34">
+        <v>55</v>
+      </c>
+      <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="34">
+        <v>56</v>
+      </c>
+      <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34">
+      <c r="D36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="34">
+        <v>57</v>
+      </c>
+      <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34">
+      <c r="D37">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="34">
+        <v>58</v>
+      </c>
+      <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34">
+      <c r="D38">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="34">
+        <v>59</v>
+      </c>
+      <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34">
+      <c r="D39">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="34">
+        <v>60</v>
+      </c>
+      <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34">
+      <c r="D40">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="34">
+        <v>61</v>
+      </c>
+      <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34">
+      <c r="D41">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="34">
+        <v>62</v>
+      </c>
+      <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34">
+      <c r="D42">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="34">
+        <v>63</v>
+      </c>
+      <c r="B43">
         <v>1</v>
       </c>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34">
+      <c r="D43">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="34">
+        <v>64</v>
+      </c>
+      <c r="B44">
         <v>1</v>
       </c>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34">
+      <c r="D44">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" s="34">
+        <v>65</v>
+      </c>
+      <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34">
+      <c r="D45">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="34">
+        <v>66</v>
+      </c>
+      <c r="B46">
         <v>1</v>
       </c>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34">
+      <c r="D46">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" s="34">
+        <v>67</v>
+      </c>
+      <c r="B47">
         <v>1</v>
       </c>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34">
+      <c r="D47">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34">
+        <v>68</v>
+      </c>
+      <c r="C48">
         <v>1</v>
       </c>
-      <c r="D48" s="34">
+      <c r="D48">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="34">
+        <v>69</v>
+      </c>
+      <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34">
+      <c r="D49">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B50" s="34">
+        <v>70</v>
+      </c>
+      <c r="B50">
         <v>1</v>
       </c>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34">
+      <c r="D50">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B51" s="34">
+        <v>71</v>
+      </c>
+      <c r="B51">
         <v>1</v>
       </c>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34">
+      <c r="D51">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" s="34">
+        <v>86</v>
+      </c>
+      <c r="B52">
         <v>40</v>
       </c>
-      <c r="C52" s="34">
+      <c r="C52">
         <v>7</v>
       </c>
-      <c r="D52" s="34">
+      <c r="D52">
         <v>47</v>
       </c>
     </row>

</xml_diff>